<commit_message>
update data and python notebook
</commit_message>
<xml_diff>
--- a/new-data-graph2.xlsx
+++ b/new-data-graph2.xlsx
@@ -8,14 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/surya/Documents/physics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B33F957C-57D7-9C46-96A8-851518E84FC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674EFC1D-6C3C-8843-99F5-61276909E689}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" xr2:uid="{C1C17879-08AB-EF43-B8F0-3E4AD4D9ED7C}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{C1C17879-08AB-EF43-B8F0-3E4AD4D9ED7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Chart1" sheetId="3" r:id="rId2"/>
+    <sheet name="Chart2" sheetId="4" r:id="rId3"/>
+    <sheet name="Chart3" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$24</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -47,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -85,7 +91,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -137,14 +143,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>Graph 1. Position is directly proportional to time</a:t>
+              <a:t>Graph 1. Position is quadratically proportional to time</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:endParaRPr lang="en-US" sz="1600" b="1">
               <a:effectLst/>
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -156,8 +162,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.34927448480038525"/>
-          <c:y val="0.93232830820770529"/>
+          <c:x val="0.20477044246855106"/>
+          <c:y val="0.57189774005875538"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -196,10 +202,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14926594740267479"/>
-          <c:y val="2.1316820322082854E-2"/>
-          <c:w val="0.83102458522959854"/>
-          <c:h val="0.84011925896530837"/>
+          <c:x val="0.21896623530415321"/>
+          <c:y val="0.11476178363230818"/>
+          <c:w val="0.74738432116854248"/>
+          <c:h val="0.38624367544168842"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -245,83 +251,23 @@
             <c:spPr>
               <a:ln w="19050" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-                <a:headEnd type="triangle"/>
-                <a:tailEnd type="triangle"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
                 <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="2.0737375268635106E-2"/>
-                  <c:y val="0.23949946583310253"/>
+                  <c:x val="-0.22833068226864234"/>
+                  <c:y val="0.10390214824173717"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1800" baseline="0">
-                        <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <a:t>y = 2.828x - 0.101</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="1800" baseline="0">
-                        <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1800" baseline="0">
-                        <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                        <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <a:t>R² = 0.9971</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1800">
-                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -335,7 +281,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -356,7 +302,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.11362999999999999</c:v>
@@ -425,7 +371,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1.4999999999999999E-2</c:v>
@@ -493,7 +439,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B835-4244-B79D-C3AB0C99B295}"/>
+              <c16:uniqueId val="{00000001-ACAF-8046-9832-4C5E6854BD87}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -605,7 +551,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -725,8 +671,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="9.0600226500566258E-3"/>
-              <c:y val="0.45527928355689207"/>
+              <c:x val="5.0772174859878266E-3"/>
+              <c:y val="0.29508793124430488"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -758,7 +704,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -816,12 +762,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -836,11 +777,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -878,21 +814,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1">
+              <a:rPr lang="en-US" sz="1600" b="1">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
               <a:t>Graph</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t> 2. Velocity increases with acceleration then remains constant when the coefficient of kinetic friction is equal to zero (</a:t>
+              <a:t> 2. Velocity remains constant when the coefficient of kinetic friction is equal to zero (</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -900,7 +836,7 @@
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="1" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="1" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -908,7 +844,7 @@
               <a:t>μ</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="1" u="none" strike="noStrike" baseline="-25000">
+              <a:rPr lang="en-US" sz="1600" b="1" i="1" u="none" strike="noStrike" baseline="-25000">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -916,7 +852,7 @@
               <a:t>k</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -924,13 +860,13 @@
               <a:t> = 0 </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t>)</a:t>
+              <a:t>) in relation to time</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:endParaRPr lang="en-US" sz="1600" b="1">
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:endParaRPr>
@@ -941,8 +877,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18899379921259843"/>
-          <c:y val="0.86885245901639341"/>
+          <c:x val="0.1451843473000618"/>
+          <c:y val="0.56317504442265509"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -984,7 +920,7 @@
           <c:x val="0.18952490157480315"/>
           <c:y val="7.5993933135407254E-2"/>
           <c:w val="0.78390639763779524"/>
-          <c:h val="0.67689541112688778"/>
+          <c:h val="0.42166960948256604"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1080,7 +1016,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.11362999999999999</c:v>
@@ -1149,7 +1085,7 @@
             <c:numRef>
               <c:f>Sheet1!$C$2:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.19400000000000001</c:v>
@@ -1217,7 +1153,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0196-204D-AEBF-95DFAB69AB31}"/>
+              <c16:uniqueId val="{00000001-F8E1-164F-9F1A-610DEE7511F5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1337,7 +1273,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1477,7 +1413,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1535,12 +1471,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1555,11 +1486,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -1597,21 +1523,21 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1">
+              <a:rPr lang="en-US" sz="1600" b="1">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
               <a:t>Graph 3.</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
-              <a:t> Acceleration is inversely proportional to time </a:t>
+              <a:t> Acceleration data points are precise and acceleration is constant in relation to time </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1619,7 +1545,7 @@
               <a:t>when the coefficient of kinetic friction is equal to zero ( </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="el-GR" sz="1800" b="1" i="1" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="el-GR" sz="1600" b="1" i="1" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1627,7 +1553,7 @@
               <a:t>μ</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="1" u="none" strike="noStrike" baseline="-25000">
+              <a:rPr lang="en-US" sz="1600" b="1" i="1" u="none" strike="noStrike" baseline="-25000">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1635,7 +1561,7 @@
               <a:t>k</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:effectLst/>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
@@ -1643,20 +1569,20 @@
               <a:t> = 0)</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" sz="1800" b="1" baseline="0">
+              <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:rPr>
               <a:t> </a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1800" b="1">
+            <a:endParaRPr lang="en-US" sz="1600" b="1">
               <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:endParaRPr>
@@ -1667,8 +1593,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.20084877525413244"/>
-          <c:y val="0.901002004008016"/>
+          <c:x val="0.22075827294640551"/>
+          <c:y val="0.62349773336692338"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1710,7 +1636,7 @@
           <c:x val="0.25240993980833221"/>
           <c:y val="6.3939723051859895E-2"/>
           <c:w val="0.72362732083431847"/>
-          <c:h val="0.7749576317990311"/>
+          <c:h val="0.48112961944214516"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1768,51 +1694,10 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-6.5727462258707028E-2"/>
-                  <c:y val="-0.22989112082432581"/>
+                  <c:x val="-6.1085752251741281E-2"/>
+                  <c:y val="0.25520170316682583"/>
                 </c:manualLayout>
               </c:layout>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr>
-                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="65000"/>
-                            <a:lumOff val="35000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t>y = 10452x</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="30000"/>
-                      <a:t>2</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t> - 2504.5x + 143.48</a:t>
-                    </a:r>
-                    <a:br>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                    </a:br>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1600" b="0" baseline="0"/>
-                      <a:t>R² = 0.3952</a:t>
-                    </a:r>
-                    <a:endParaRPr lang="en-US" sz="1600" b="0"/>
-                  </a:p>
-                </c:rich>
-              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1826,7 +1711,7 @@
                 <a:lstStyle/>
                 <a:p>
                   <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                       <a:solidFill>
                         <a:schemeClr val="tx1">
                           <a:lumMod val="65000"/>
@@ -1847,7 +1732,7 @@
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>0.11362999999999999</c:v>
@@ -1916,7 +1801,7 @@
             <c:numRef>
               <c:f>Sheet1!$D$2:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1.0900000000000001</c:v>
@@ -1984,7 +1869,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B279-0C4D-AABE-E3CEDDE74536}"/>
+              <c16:uniqueId val="{00000001-2E89-3F4F-8F2C-CA07E7CFD0A2}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2064,8 +1949,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.61519436199143274"/>
-              <c:y val="0.85012671011313967"/>
+              <c:x val="0.57537533328818424"/>
+              <c:y val="0.56817052633842124"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2097,7 +1982,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2213,8 +2098,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.7229001109272425E-2"/>
-              <c:y val="0.44070645227462801"/>
+              <c:x val="1.3247029565138874E-2"/>
+              <c:y val="0.27746869971119648"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -2246,7 +2131,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2324,11 +2209,6 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -4000,32 +3880,58 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{0CBE3602-A98A-E045-BBED-133FB33DE90D}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{72CD1666-2267-AE4B-A72F-05FCC0B33ADE}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="109" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{8A37E341-11DA-B041-BB3C-3B37F0CF688E}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:to>
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6377312" cy="8562258"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FD9E5A1-C54A-5349-9190-717630BFEA0B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14030B37-671C-804F-89CB-F489BA794D22}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4039,31 +3945,26 @@
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>766763</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>195262</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>192088</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6377609" cy="8558696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{933B925C-F70C-9D45-AE17-CB0EBDD6246A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34FA4B91-3AB3-6144-B7A9-64BC03F882B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4072,36 +3973,31 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>185738</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>39688</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>456672</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>77788</xdr:rowOff>
-    </xdr:to>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="6378864" cy="8558068"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5C0C871-9C4B-7F4F-9B4D-5D422BEAADAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98CC78B0-8C8C-9E41-8DDA-9D66860D512D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
+          <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -4110,12 +4006,12 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:absoluteAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4416,15 +4312,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FD31552-86D3-3C40-9C5D-A6D7DB7D319D}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:K24"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4438,7 +4334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>0.11362999999999999</v>
       </c>
@@ -4451,20 +4347,8 @@
       <c r="D2" s="2">
         <v>1.0900000000000001</v>
       </c>
-      <c r="H2" s="2">
-        <v>0.11362999999999999</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J2" s="2">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1.0900000000000001</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>0.17902999999999999</v>
       </c>
@@ -4477,20 +4361,8 @@
       <c r="D3" s="2">
         <v>1.07</v>
       </c>
-      <c r="H3" s="2">
-        <v>0.17902999999999999</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1.07</v>
-      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>0.23039999999999999</v>
       </c>
@@ -4503,20 +4375,8 @@
       <c r="D4" s="2">
         <v>1.01</v>
       </c>
-      <c r="H4" s="2">
-        <v>0.23039999999999999</v>
-      </c>
-      <c r="I4" s="2">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0.318</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1.01</v>
-      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>0.27450999999999998</v>
       </c>
@@ -4529,20 +4389,8 @@
       <c r="D5" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="H5" s="2">
-        <v>0.27450999999999998</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="K5" s="2">
-        <v>1.1000000000000001</v>
-      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>0.31341000000000002</v>
       </c>
@@ -4555,20 +4403,8 @@
       <c r="D6" s="2">
         <v>0.98</v>
       </c>
-      <c r="H6" s="2">
-        <v>0.31341000000000002</v>
-      </c>
-      <c r="I6" s="2">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.40500000000000003</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0.98</v>
-      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>0.34893999999999997</v>
       </c>
@@ -4581,20 +4417,8 @@
       <c r="D7" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="H7" s="2">
-        <v>0.34893999999999997</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.09</v>
-      </c>
-      <c r="J7" s="2">
-        <v>0.442</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1.1200000000000001</v>
-      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>0.38152999999999998</v>
       </c>
@@ -4607,20 +4431,8 @@
       <c r="D8" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H8" s="2">
-        <v>0.38152999999999998</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.105</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0.47899999999999998</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1.1299999999999999</v>
-      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>0.4118</v>
       </c>
@@ -4633,20 +4445,8 @@
       <c r="D9" s="2">
         <v>0.97</v>
       </c>
-      <c r="H9" s="2">
-        <v>0.4118</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.51</v>
-      </c>
-      <c r="K9" s="2">
-        <v>0.97</v>
-      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>0.44041000000000002</v>
       </c>
@@ -4659,20 +4459,8 @@
       <c r="D10" s="2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="H10" s="2">
-        <v>0.44041000000000002</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.54</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1.1399999999999999</v>
-      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>0.46739999999999998</v>
       </c>
@@ -4685,20 +4473,8 @@
       <c r="D11" s="2">
         <v>1.08</v>
       </c>
-      <c r="H11" s="2">
-        <v>0.46739999999999998</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1.08</v>
-      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>0.49308000000000002</v>
       </c>
@@ -4711,20 +4487,8 @@
       <c r="D12" s="2">
         <v>0.99</v>
       </c>
-      <c r="H12" s="2">
-        <v>0.49308000000000002</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.59699999999999998</v>
-      </c>
-      <c r="K12" s="2">
-        <v>0.99</v>
-      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>0.51770000000000005</v>
       </c>
@@ -4737,20 +4501,8 @@
       <c r="D13" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H13" s="2">
-        <v>0.51770000000000005</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.18</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.623</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1.1299999999999999</v>
-      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>0.54125999999999996</v>
       </c>
@@ -4763,20 +4515,8 @@
       <c r="D14" s="2">
         <v>0.93</v>
       </c>
-      <c r="H14" s="2">
-        <v>0.54125999999999996</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="K14" s="2">
-        <v>0.93</v>
-      </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>0.56406000000000001</v>
       </c>
@@ -4789,20 +4529,8 @@
       <c r="D15" s="2">
         <v>1.03</v>
       </c>
-      <c r="H15" s="2">
-        <v>0.56406000000000001</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0.21</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="K15" s="2">
-        <v>1.03</v>
-      </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>0.58608000000000005</v>
       </c>
@@ -4815,20 +4543,8 @@
       <c r="D16" s="2">
         <v>0.85</v>
       </c>
-      <c r="H16" s="2">
-        <v>0.58608000000000005</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.69099999999999995</v>
-      </c>
-      <c r="K16" s="2">
-        <v>0.85</v>
-      </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17" s="2">
         <v>0.60750999999999999</v>
       </c>
@@ -4841,20 +4557,8 @@
       <c r="D17" s="2">
         <v>1.21</v>
       </c>
-      <c r="H17" s="2">
-        <v>0.60750999999999999</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="K17" s="2">
-        <v>1.21</v>
-      </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>0.62819999999999998</v>
       </c>
@@ -4867,20 +4571,8 @@
       <c r="D18" s="2">
         <v>1.18</v>
       </c>
-      <c r="H18" s="2">
-        <v>0.62819999999999998</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.255</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="K18" s="2">
-        <v>1.18</v>
-      </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19" s="2">
         <v>0.64822000000000002</v>
       </c>
@@ -4893,20 +4585,8 @@
       <c r="D19" s="2">
         <v>0.99</v>
       </c>
-      <c r="H19" s="2">
-        <v>0.64822000000000002</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.27</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.75900000000000001</v>
-      </c>
-      <c r="K19" s="2">
-        <v>0.99</v>
-      </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="2">
         <v>0.66774</v>
       </c>
@@ -4919,20 +4599,8 @@
       <c r="D20" s="2">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H20" s="2">
-        <v>0.66774</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.28499999999999998</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.78</v>
-      </c>
-      <c r="K20" s="2">
-        <v>1.1299999999999999</v>
-      </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="2">
         <v>0.68671000000000004</v>
       </c>
@@ -4945,20 +4613,8 @@
       <c r="D21" s="2">
         <v>1.1200000000000001</v>
       </c>
-      <c r="H21" s="2">
-        <v>0.68671000000000004</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.80100000000000005</v>
-      </c>
-      <c r="K21" s="2">
-        <v>1.1200000000000001</v>
-      </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>0.70518999999999998</v>
       </c>
@@ -4971,20 +4627,8 @@
       <c r="D22" s="2">
         <v>1</v>
       </c>
-      <c r="H22" s="2">
-        <v>0.70518999999999998</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.315</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.82099999999999995</v>
-      </c>
-      <c r="K22" s="2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="A23" s="2">
         <v>0.72326000000000001</v>
       </c>
@@ -4997,20 +4641,8 @@
       <c r="D23" s="2">
         <v>1.02</v>
       </c>
-      <c r="H23" s="2">
-        <v>0.72326000000000001</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.33</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="K23" s="2">
-        <v>1.02</v>
-      </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4">
       <c r="A24" s="2">
         <v>0.74095</v>
       </c>
@@ -5021,23 +4653,12 @@
         <v>0.85699999999999998</v>
       </c>
       <c r="D24" s="2">
-        <v>0.95</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.74095</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.85699999999999998</v>
-      </c>
-      <c r="K24" s="2">
         <v>0.95</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -5045,13 +4666,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112A8F1C-4189-AB41-8636-40285C1DDA1C}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView topLeftCell="A27" zoomScale="60" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>